<commit_message>
Testes realizados + Resultados completos
</commit_message>
<xml_diff>
--- a/results/bubble_sort_details.xlsx
+++ b/results/bubble_sort_details.xlsx
@@ -14,6 +14,7 @@
     <sheet name="N=80000" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="N=100000" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="N=150000" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="N=200000" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1146,4 +1147,109 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Execução</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1915306.9410 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1860100.6758 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1919220.2342 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2011586.7720 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026716.4772 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1946586.2200 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Desvio Padrão</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>70450.2833 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>